<commit_message>
Some script documentation changes.
</commit_message>
<xml_diff>
--- a/Display/TestingLogs/concurrent.xlsx
+++ b/Display/TestingLogs/concurrent.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\17Fall\SeniorDesign\SolarCarProject\Display\TestLogs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\17Fall\SeniorDesign\SolarCarProject\Display\TestingLogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -144,36 +144,22 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" b="1">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>CPU Usage</a:t>
+              <a:rPr lang="en-US" sz="1600" b="1"/>
+              <a:t>CPU Usage by Seconds</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" b="1" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t> by Seconds</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" b="1">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -190,13 +176,16 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -16905,21 +16894,20 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
-                    </a:solidFill>
-                  </a:rPr>
+                  <a:rPr lang="en-US"/>
                   <a:t>Time (seconds)</a:t>
                 </a:r>
               </a:p>
@@ -16938,13 +16926,16 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:sysClr val="windowText" lastClr="000000"/>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="en-US"/>
@@ -16973,16 +16964,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -17020,36 +17011,22 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
-                    </a:solidFill>
-                  </a:rPr>
-                  <a:t>%</a:t>
+                  <a:rPr lang="en-US"/>
+                  <a:t>% Usage of one CPU Core</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
-                    </a:solidFill>
-                  </a:rPr>
-                  <a:t> Usage of one CPU Core</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US">
-                  <a:solidFill>
-                    <a:sysClr val="windowText" lastClr="000000"/>
-                  </a:solidFill>
-                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -17066,13 +17043,16 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:sysClr val="windowText" lastClr="000000"/>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="en-US"/>
@@ -17101,13 +17081,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -17140,13 +17123,16 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -17179,7 +17165,10 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1200">
+          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -18078,7 +18067,7 @@
   <dimension ref="A1:P176"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="T23" sqref="T23"/>
+      <selection activeCell="Z22" sqref="Z22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>